<commit_message>
Update 13C-MFA files (run and result) for SC and IO under WT-batch and chemostats
</commit_message>
<xml_diff>
--- a/mfa/I_orientalis/result_files/batch/mfa.xlsx
+++ b/mfa/I_orientalis/result_files/batch/mfa.xlsx
@@ -504,16 +504,16 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.122083 0.015364 0.241366 0.138691 0.138775 0.241265 0.015036 0.117412</t>
+          <t>0.122092 0.015246 0.241426 0.138592 0.138674 0.241327 0.014921 0.117462</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>-0.12474074074074214 1.6417777777777776 -0.363407407407409 0.38177777777777716 2.455703703703705 -1.6130370370370384 1.65362962962963 0.41155555555555595</t>
+          <t>-0.12340740740740747 1.6242962962962961 -0.35451851851851945 0.36711111111110817 2.4407407407407393 -1.6038518518518523 1.6365925925925928 0.41896296296296254</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>14.52505182990399</v>
+        <v>14.2975431989026</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -521,7 +521,7 @@
         </is>
       </c>
       <c r="I2" t="n">
-        <v>0.5125277142857143</v>
+        <v>0.5124235714285714</v>
       </c>
     </row>
     <row r="3">
@@ -547,16 +547,16 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.231929 0.020551 0.243897 0.24378 0.020606 0.231867</t>
+          <t>0.231966 0.020406 0.243868 0.243754 0.02046 0.231906</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2.1133333333333333 -0.5665185185185186 0.05555555555555766 -1.1456296296296282 -0.6924444444444446 -0.8561481481481491</t>
+          <t>2.118814814814816 -0.5880000000000001 0.05125925925926118 -1.1494814814814798 -0.7140740740740743 -0.8503703703703697</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>7.31514363786008</v>
+        <v>7.392086957475994</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -564,7 +564,7 @@
         </is>
       </c>
       <c r="I3" t="n">
-        <v>0.4962888</v>
+        <v>0.4961548</v>
       </c>
     </row>
     <row r="4">
@@ -590,16 +590,16 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.480864 0.008352 0.008253 0.068163 0.008185 0.005856 0.442819</t>
+          <t>0.480857 0.008462 0.008461 0.067842 0.008393 0.00597 0.442873</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>-0.03779732811990587 0.5607689801238188 0.5390192245030955 1.2981427174975562 0.0423590746171391 -0.39532420984033884 -0.1749755620723349</t>
+          <t>-0.03836754643206249 0.5697295536005214 0.5559628543499511 1.2719941348973605 0.05930270446399474 -0.3860377973281199 -0.1705767350928629</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>2.480298695868808</v>
+        <v>2.434766021772926</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -607,7 +607,7 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>0.4913801666666667</v>
+        <v>0.491595</v>
       </c>
     </row>
     <row r="5">
@@ -633,16 +633,16 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.136838 0.132872 0.246425 0.243889 0.132754 0.111713</t>
+          <t>0.136833 0.132954 0.246391 0.24388 0.132819 0.111625</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>-0.03466666666666844 0.6493333333333331 -0.6459259259259222 -0.24296296296296335 1.5177777777777783 -0.5782222222222207</t>
+          <t>-0.03540740740740581 0.661481481481481 -0.6509629629629602 -0.2442962962962939 1.5274074074074053 -0.5912592592592585</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>3.537077179698212</v>
+        <v>3.60480579423867</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -650,7 +650,7 @@
         </is>
       </c>
       <c r="I5" t="n">
-        <v>0.4893940000000001</v>
+        <v>0.4893554</v>
       </c>
     </row>
     <row r="6">
@@ -676,16 +676,16 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.486448 0.024039 0.02416 0.486319</t>
+          <t>0.486456 0.023915 0.024033 0.48633</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2.359555555555551 1.778962962962963 1.4897777777777779 -2.522222222222224</t>
+          <t>2.3607407407407375 1.7605925925925925 1.4709629629629628 -2.520592592592597</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>17.31325440877914</v>
+        <v>17.18990217832648</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -693,7 +693,7 @@
         </is>
       </c>
       <c r="I6" t="n">
-        <v>0.5104386666666667</v>
+        <v>0.5103236666666667</v>
       </c>
     </row>
     <row r="7">
@@ -719,16 +719,16 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.068405 0.124995 0.194554 0.248437 0.188031 0.123365 0.053736</t>
+          <t>0.068405 0.124988 0.194557 0.248416 0.188076 0.123352 0.053709</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>0.0879999999999996 -1.3201481481481485 -0.7533333333333343 -0.05318518518518492 0.9608888888888877 0.9770370370370376 0.32637037037036987</t>
+          <t>0.0879999999999996 -1.3211851851851846 -0.7528888888888894 -0.05629629629629503 0.9675555555555528 0.9751111111111118 0.32237037037037</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>4.305301355281207</v>
+        <v>4.314213333333328</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -736,7 +736,7 @@
         </is>
       </c>
       <c r="I7" t="n">
-        <v>0.4917965</v>
+        <v>0.491778</v>
       </c>
     </row>
     <row r="8">
@@ -762,16 +762,16 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.249058 0.233915 0.049198 0.255377 0.224407</t>
+          <t>0.249057 0.233955 0.049316 0.255291 0.224433</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0.00474074074074137 -0.14711111111111022 2.2831111111111113 0.12340740740741159 -0.4930370370370367</t>
+          <t>0.004592592592593074 -0.14118518518518658 2.3005925925925927 0.11066666666666632 -0.4891851851851851</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>5.492575407407409</v>
+        <v>5.56422988203018</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -779,7 +779,7 @@
         </is>
       </c>
       <c r="I8" t="n">
-        <v>0.4990175</v>
+        <v>0.499048</v>
       </c>
     </row>
     <row r="9">
@@ -805,16 +805,16 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0.124409 0.101731 0.198776 0.198172 0.196311 0.101042 0.077595</t>
+          <t>0.124406 0.101787 0.198705 0.198276 0.196264 0.101071 0.077529</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>0.03437037037037185 -0.5026666666666657 -0.7758518518518506 -0.5711111111111148 1.5211851851851892 0.6560000000000002 -0.6528888888888901</t>
+          <t>0.03392592592592696 -0.4943703703703693 -0.7863703703703714 -0.5557037037037044 1.5142222222222235 0.6602962962962946 -0.6626666666666674</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>4.35257336625516</v>
+        <v>4.340725245541842</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="I9" t="n">
-        <v>0.4749705</v>
+        <v>0.4749350000000001</v>
       </c>
     </row>
     <row r="10">
@@ -848,16 +848,16 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0.064315 0.126164 0.196866 0.2514 0.190274 0.124836 0.054377</t>
+          <t>0.064316 0.126157 0.196869 0.251379 0.190319 0.124823 0.054349</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>0.025918142699889457 -0.38667066946862866 -0.3086160312218529 -0.4029820874612231 0.06374462123486427 1.3827679375562891 0.44961473031121824</t>
+          <t>0.02601821274892388 -0.38737115981186965 -0.30831582107475236 -0.40508355849094324 0.0682477734414078 1.381467026918843 0.44681276893825717</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>2.526088325872941</v>
+        <v>2.522635253263295</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -865,7 +865,7 @@
         </is>
       </c>
       <c r="I10" t="n">
-        <v>0.4976056666666667</v>
+        <v>0.4975861666666667</v>
       </c>
     </row>
     <row r="11">
@@ -891,16 +891,16 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>0.500357 0.023771 0.02274 0.468583</t>
+          <t>0.500363 0.02359 0.022559 0.468601</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>-0.04330908475723177 1.324592567529465 -0.4088422714712683 -0.001127840748884255</t>
+          <t>-0.04297073253256868 1.3143856087520442 -0.4190492302486889 -0.00011278407488873853</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>1.92357442174335</v>
+        <v>1.905058282441134</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
@@ -908,7 +908,7 @@
         </is>
       </c>
       <c r="I11" t="n">
-        <v>0.4916666666666667</v>
+        <v>0.4915036666666666</v>
       </c>
     </row>
     <row r="12">
@@ -934,16 +934,16 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>0.308836 0.016968 0.017589 0.381607 0.017561 0.015946 0.293258</t>
+          <t>0.30884 0.016913 0.017531 0.381662 0.017503 0.015887 0.293207</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>-0.11718518518518313 1.719851851851852 2.4054814814814818 -0.3986666666666665 1.518074074074074 2.3623703703703702 0.17896296296296924</t>
+          <t>-0.11659259259258994 1.711703703703704 2.3968888888888893 -0.3905185185185143 1.5094814814814814 2.3536296296296295 0.17140740740741026</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>16.83426943209877</v>
+        <v>16.68859173662551</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
@@ -951,7 +951,7 @@
         </is>
       </c>
       <c r="I12" t="n">
-        <v>0.5177481666666667</v>
+        <v>0.5176083333333333</v>
       </c>
     </row>
     <row r="13">
@@ -977,16 +977,16 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>0.236503 0.217817 0.115754 0.232115 0.198396</t>
+          <t>0.236503 0.217824 0.115797 0.232039 0.198452</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>-0.014814814814817296 0.3337777777777785 0.22859259259259299 -0.12562962962963192 -0.3352592592592615</t>
+          <t>-0.014814814814817296 0.3348148148148125 0.23496296296296357 -0.1368888888888901 -0.3269629629629651</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>0.2920632318244198</v>
+        <v>0.2931713799725657</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
@@ -994,7 +994,7 @@
         </is>
       </c>
       <c r="I13" t="n">
-        <v>0.4848135</v>
+        <v>0.48483575</v>
       </c>
     </row>
     <row r="14">
@@ -1020,16 +1020,16 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>0.503275 0.012407 0.011958 0.489451</t>
+          <t>0.503274 0.012434 0.011985 0.48945</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>-0.05185185185184614 1.5696296296296297 1.0257777777777777 -0.011555555555550665</t>
+          <t>-0.05199999999999855 1.57362962962963 1.029777777777778 -0.011703703703703073</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>3.518779368998628</v>
+        <v>3.539593459533608</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
@@ -1037,7 +1037,7 @@
         </is>
       </c>
       <c r="I14" t="n">
-        <v>0.5015586666666667</v>
+        <v>0.5015846666666667</v>
       </c>
     </row>
     <row r="15">
@@ -1063,16 +1063,16 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>0.452653 0.006674 0.008148 0.067655 0.008124 0.005813 0.439524</t>
+          <t>0.452645 0.006784 0.008354 0.067335 0.00833 0.005925 0.439563</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>-0.0071111111111099995 0.09896296296296299 0.3828148148148149 -1.441629629629628 -0.7140740740740743 -0.24637037037037043 0.23718518518518802</t>
+          <t>-0.00829629629629637 0.11525925925925927 0.41333333333333333 -1.4890370370370356 -0.6835555555555556 -0.22977777777777783 0.24296296296295924</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>2.861544362139915</v>
+        <v>2.980506293552806</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
@@ -1080,7 +1080,7 @@
         </is>
       </c>
       <c r="I15" t="n">
-        <v>0.48744</v>
+        <v>0.4876366666666667</v>
       </c>
     </row>
     <row r="16">
@@ -1106,16 +1106,16 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>0.129452 0.133538 0.248516 0.245968 0.133885 0.112665</t>
+          <t>0.129447 0.133621 0.248482 0.245961 0.133952 0.112577</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>-0.001333333333330555 0.03896296296296081 -0.6161481481481476 -0.08844444444444655 1.297481481481484 -0.034370370370369795</t>
+          <t>-0.0020740740740720362 0.05125925925925707 -0.6211851851851814 -0.08948148148148051 1.3074074074074074 -0.04740740740740753</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>2.073620367626892</v>
+        <v>2.108071374485591</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -1123,7 +1123,7 @@
         </is>
       </c>
       <c r="I16" t="n">
-        <v>0.4934678</v>
+        <v>0.4934322</v>
       </c>
     </row>
     <row r="17">
@@ -1149,16 +1149,16 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.130608 0.133486 0.248292 0.245746 0.133764 0.112563</t>
+          <t>0.130604 0.133568 0.248257 0.245736 0.13383 0.112475</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>-0.03688888888888878 0.6860740740740735 -0.5130370370370362 -0.4210370370370387 1.7768888888888876 -0.8314074074074083</t>
+          <t>-0.03748148148148196 0.6982222222222215 -0.5182222222222224 -0.42251851851851757 1.7866666666666668 -0.844444444444444</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>4.761110013717418</v>
+        <v>4.841259500685869</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
@@ -1166,7 +1166,7 @@
         </is>
       </c>
       <c r="I17" t="n">
-        <v>0.4930358</v>
+        <v>0.4929970000000001</v>
       </c>
     </row>
     <row r="18">
@@ -1192,16 +1192,16 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>0.475048 0.049973 0.474944</t>
+          <t>0.475703 0.049475 0.474313</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>0.9983462532299772 -0.0038242894056849932 -0.9981395348837238</t>
+          <t>1.0660465116279059 -0.055297157622739096 -1.063359173126617</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>1.992992397625688</v>
+        <v>2.270245671667704</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
@@ -1209,7 +1209,7 @@
         </is>
       </c>
       <c r="I18" t="n">
-        <v>0.4999305</v>
+        <v>0.4990505</v>
       </c>
     </row>
     <row r="19">
@@ -1235,16 +1235,16 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0.495513 0.023496 0.022384 0.46122</t>
+          <t>0.495519 0.023318 0.022206 0.461232</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>-0.005925925925931852 0.17748148148148166 0.22933333333333344 -0.013777777777770997</t>
+          <t>-0.0050370370370420746 0.1511111111111111 0.20296296296296293 -0.011999999999999665</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>0.08431839780521261</v>
+        <v>0.06419790397805215</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
@@ -1252,7 +1252,7 @@
         </is>
       </c>
       <c r="I19" t="n">
-        <v>0.4839746666666667</v>
+        <v>0.4838086666666667</v>
       </c>
     </row>
     <row r="20">
@@ -1278,16 +1278,16 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>0.129823 0.116639 0.145371 0.233622 0.134907 0.125659 0.106744</t>
+          <t>0.129824 0.116631 0.145358 0.233631 0.13495 0.125599 0.106775</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>-0.06666666666666755 1.106962962962964 -3.3755555555555556 2.131555555555553 -2.3971851851851853 1.7146666666666648 -0.18562962962962817</t>
+          <t>-0.06651851851851925 1.1057777777777775 -3.3774814814814835 2.1328888888888877 -2.3908148148148167 1.7057777777777752 -0.18103703703703716</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>25.88875279012344</v>
+        <v>25.84221309190673</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
@@ -1295,7 +1295,7 @@
         </is>
       </c>
       <c r="I20" t="n">
-        <v>0.4861056666666667</v>
+        <v>0.4861141666666666</v>
       </c>
     </row>
     <row r="21">
@@ -1321,16 +1321,16 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>0.137152 0.015275 0.362988 0.028413 0.362958 0.014202 0.1208</t>
+          <t>0.137161 0.015137 0.363012 0.028136 0.362982 0.014064 0.120812</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>-0.10162962962962847 1.5905185185185187 -1.558666666666667 2.9878518518518518 0.9099259259259231 1.3617777777777775 1.001037037037037</t>
+          <t>-0.1002962962962938 1.570074074074074 -1.555111111111108 2.9468148148148146 0.9134814814814822 1.3413333333333333 1.0028148148148144</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>17.58125726200274</v>
+        <v>17.2165411467764</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
@@ -1338,7 +1338,7 @@
         </is>
       </c>
       <c r="I21" t="n">
-        <v>0.5123553333333334</v>
+        <v>0.5121148333333334</v>
       </c>
     </row>
     <row r="22">
@@ -1364,16 +1364,16 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>0.088499 0.101401 0.223943 0.200796 0.223908 0.100322 0.072102</t>
+          <t>0.088492 0.101513 0.223769 0.201013 0.223734 0.100432 0.072065</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>-0.007319023310167169 0.15431453348914517 -1.6095085798634603 2.0649486438280333 -0.6109846854050064 0.6501629866535455 0.0331508702872254</t>
+          <t>-0.007749554093117727 0.16120302601636094 -1.6202103450396708 2.0782950980995136 -0.621686450581217 0.6569284703856324 0.030875207577341933</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>7.675510488864028</v>
+        <v>7.789440884625933</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
@@ -1381,7 +1381,7 @@
         </is>
       </c>
       <c r="I22" t="n">
-        <v>0.4969215</v>
+        <v>0.4969293333333333</v>
       </c>
     </row>
     <row r="23">
@@ -1407,16 +1407,16 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0.235576 0.22414 0.081748 0.243012 0.21554</t>
+          <t>0.235512 0.224203 0.081738 0.242977 0.215588</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>0.2558518518518528 -0.16385185185185125 0.03866666666666627 0.034814814814816734 -0.16311111111110976</t>
+          <t>0.24637037037037005 -0.1545185185185168 0.03718518518518537 0.029629629629630477 -0.15599999999999975</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>0.1216200164609053</v>
+        <v>0.1111709849108361</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
@@ -1424,7 +1424,7 @@
         </is>
       </c>
       <c r="I23" t="n">
-        <v>0.494708</v>
+        <v>0.4947405</v>
       </c>
     </row>
     <row r="24">
@@ -1450,16 +1450,16 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>0.134864 0.236488 0.138719 0.14926 0.235123 0.109973</t>
+          <t>0.134866 0.236453 0.138793 0.149274 0.235093 0.109985</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>-0.004148148148148185 0.023703703703702738 2.3545185185185193 0.9157037037037026 -1.4280000000000013 -1.2059259259259252</t>
+          <t>-0.003851851851851592 0.01851851851851648 2.365481481481481 0.9177777777777746 -1.4324444444444462 -1.2041481481481475</t>
         </is>
       </c>
       <c r="G24" t="n">
-        <v>9.876291138545957</v>
+        <v>9.940046310013713</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
@@ -1467,7 +1467,7 @@
         </is>
       </c>
       <c r="I24" t="n">
-        <v>0.4904126</v>
+        <v>0.4904316</v>
       </c>
     </row>
     <row r="25">
@@ -1493,16 +1493,16 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>0.122299 0.135261 0.25266 0.250081 0.136124 0.114549</t>
+          <t>0.122294 0.135346 0.252626 0.250074 0.136192 0.11446</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>-0.017185185185183867 0.3536296296296297 -1.7959999999999992 0.19955555555555365 1.2797037037037047 1.6060740740740747</t>
+          <t>-0.01792592592592535 0.3662222222222225 -1.8010370370370332 0.19851851851851968 1.2897777777777806 1.5928888888888906</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>7.607903165980797</v>
+        <v>7.618405794238683</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
@@ -1510,7 +1510,7 @@
         </is>
       </c>
       <c r="I25" t="n">
-        <v>0.501613</v>
+        <v>0.5015776000000001</v>
       </c>
     </row>
     <row r="26">
@@ -1536,16 +1536,16 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>0.503949 0.012476 0.011824 0.483837</t>
+          <t>0.503948 0.012503 0.01185 0.483835</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>-0.04237037037037163 1.285925925925926 0.5493333333333332 -0.002370370370364517</t>
+          <t>-0.042518518518524034 1.289925925925926 0.5531851851851851 -0.00266666666666111</t>
         </is>
       </c>
       <c r="G26" t="n">
-        <v>1.957173465020576</v>
+        <v>1.971737679012346</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
@@ -1553,7 +1553,7 @@
         </is>
       </c>
       <c r="I26" t="n">
-        <v>0.4958783333333334</v>
+        <v>0.4959026666666667</v>
       </c>
     </row>
     <row r="27">
@@ -1579,16 +1579,16 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>0.112245 0.031036 0.096441 0.148294 0.123838 0.123838 0.148292 0.096354 0.029056 0.092125</t>
+          <t>0.112247 0.031014 0.096473 0.148261 0.123846 0.123846 0.148259 0.096387 0.029036 0.092149</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>0.03674074074074048 -0.3700740740740741 -0.02799999999999922 -1.3540740740740713 -2.383259259259258 3.4059259259259274 0.001925925925927852 0.4019259259259249 0.034074074074073715 0.47985185185185064</t>
+          <t>0.03703703703703707 -0.3733333333333336 -0.02325925925925785 -1.358962962962961 -2.3820740740740733 3.407111111111112 -0.0029629629629618144 0.4068148148148146 0.03111111111111087 0.4834074074074057</t>
         </is>
       </c>
       <c r="G27" t="n">
-        <v>19.64582841152263</v>
+        <v>19.67091156104252</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
@@ -1596,7 +1596,7 @@
         </is>
       </c>
       <c r="I27" t="n">
-        <v>0.489905</v>
+        <v>0.4899165555555556</v>
       </c>
     </row>
     <row r="28">
@@ -1622,16 +1622,16 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>0.101532 0.030449 0.098637 0.151759 0.126732 0.126732 0.151758 0.098606 0.029736 0.094278</t>
+          <t>0.101534 0.030426 0.098671 0.151725 0.12674 0.12674 0.151724 0.09864 0.029715 0.094302</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>0.018171273922288202 -0.16586120239706156 -0.39976802629035385 -1.2354533152909326 0.008505702687029262 0.4477092596172445 0.3282427991494307 -0.13106514595012528 0.9945872801082541 1.1226560989754495</t>
+          <t>0.018364585346993596 -0.16808428378117124 -0.3964817320703662 -1.2387396095109215 0.009278948385848152 0.4484825053160634 0.3249565049294417 -0.12777885173013628 0.9925575101488495 1.1249758360719115</t>
         </is>
       </c>
       <c r="G28" t="n">
-        <v>4.288997412885511</v>
+        <v>4.294151032687714</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
@@ -1639,7 +1639,7 @@
         </is>
       </c>
       <c r="I28" t="n">
-        <v>0.5011964444444446</v>
+        <v>0.5012072222222222</v>
       </c>
     </row>
     <row r="29">
@@ -1665,16 +1665,16 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>0.129436 0.134286 0.249988 0.247427 0.134679 0.113333</t>
+          <t>0.129432 0.13437 0.249954 0.247419 0.134746 0.113245</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>-0.036444444444443884 0.6942222222222216 -1.2936296296296323 -0.14251851851851713 1.3268148148148136 0.8069629629629641</t>
+          <t>-0.03703703703703707 0.7066666666666661 -1.2986666666666662 -0.1437037037037035 1.3367407407407412 0.7939259259259264</t>
         </is>
       </c>
       <c r="G29" t="n">
-        <v>4.58868861454047</v>
+        <v>4.625129569272977</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
@@ -1682,7 +1682,7 @@
         </is>
       </c>
       <c r="I29" t="n">
-        <v>0.4963848</v>
+        <v>0.4963488</v>
       </c>
     </row>
     <row r="30">
@@ -1708,16 +1708,16 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>0.444914 0.0571 0.056786 0.435258</t>
+          <t>0.444894 0.057697 0.05725 0.435145</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>-0.011523687580025286 0.36246265471617556 -1.0915492957746482 0.1065941101152339</t>
+          <t>-0.013657703798544758 0.4261630388390949 -1.0420401195049087 0.09453691848058023</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>1.334354140856729</v>
+        <v>1.276586308159229</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
@@ -1725,7 +1725,7 @@
         </is>
       </c>
       <c r="I30" t="n">
-        <v>0.4921486666666666</v>
+        <v>0.492544</v>
       </c>
     </row>
     <row r="31">
@@ -1751,16 +1751,16 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>0.192474 0.178446 0.286328 0.18032 0.166765</t>
+          <t>0.192472 0.17849 0.286205 0.180368 0.166869</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>-0.014222222222219999 0.3423703703703674 -1.0287407407407334 0.9090370370370374 0.43348148148147914</t>
+          <t>-0.01451851851851659 0.3488888888888883 -1.0469629629629615 0.9161481481481474 0.4488888888888855</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>2.189981783264728</v>
+        <v>2.258894353909457</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
@@ -1768,7 +1768,7 @@
         </is>
       </c>
       <c r="I31" t="n">
-        <v>0.4897805</v>
+        <v>0.48987</v>
       </c>
     </row>
     <row r="32">
@@ -1794,16 +1794,16 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>0.045379 0.021656 0.090839 0.093235 0.116937 0.139114 0.139114 0.116937 0.093234 0.090809 0.021111 0.04085</t>
+          <t>0.045376 0.021679 0.090847 0.093239 0.11697 0.139099 0.139098 0.116962 0.093218 0.090799 0.021114 0.040815</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>-0.05318518518518492 0.4948148148148152 -0.9491851851851846 -0.4025185185185181 -0.543851851851853 -0.34651851851851967 0.54948148148148 0.48281481481481453 0.5543703703703697 -0.19007407407407295 0.6238518518518523 1.1451851851851853</t>
+          <t>-0.05362962962962981 0.49822222222222246 -0.9480000000000003 -0.4019259259259249 -0.5389629629629633 -0.34874074074074 0.5471111111111114 0.4865185185185178 0.551999999999999 -0.19155555555555387 0.6242962962962967 1.1400000000000001</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>4.305628905349793</v>
+        <v>4.290225382716048</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
@@ -1811,7 +1811,7 @@
         </is>
       </c>
       <c r="I32" t="n">
-        <v>0.5021102727272727</v>
+        <v>0.5020751818181819</v>
       </c>
     </row>
     <row r="33">
@@ -1837,16 +1837,16 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>0.098866 0.030092 0.098169 0.151052 0.126143 0.126143 0.151052 0.098147 0.029597 0.093839</t>
+          <t>0.098868 0.030069 0.098202 0.151018 0.12615 0.12615 0.151018 0.098181 0.029576 0.093863</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>0.02014814814814774 -0.2051851851851848 0.039111111111111166 -0.5225185185185188 -0.37511111111111206 0.007555555555554888 -0.22266666666666732 0.9580740740740742 0.09422222222222187 0.6656296296296312</t>
+          <t>0.02044444444444433 -0.20859259259259252 0.043999999999998776 -0.5275555555555527 -0.374074074074074 0.008592592592592962 -0.22770370370370116 0.9631111111111121 0.09111111111111125 0.6691851851851862</t>
         </is>
       </c>
       <c r="G33" t="n">
-        <v>1.877254628257891</v>
+        <v>1.899726990397804</v>
       </c>
       <c r="H33" t="inlineStr">
         <is>
@@ -1854,7 +1854,7 @@
         </is>
       </c>
       <c r="I33" t="n">
-        <v>0.4988378888888889</v>
+        <v>0.4988474444444445</v>
       </c>
     </row>
     <row r="34">
@@ -1880,16 +1880,16 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>0.243574 0.021365 0.249413 0.249286 0.021071 0.237104</t>
+          <t>0.243582 0.021216 0.249401 0.249277 0.020923 0.23716</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>-0.10325925925925562 1.8842962962962961 0.19511111111110888 -0.2648888888888906 1.6582222222222223 -0.13792592592592406</t>
+          <t>-0.10207407407407336 1.8622222222222222 0.1933333333333334 -0.2662222222222253 1.6362962962962964 -0.12962962962962768</t>
         </is>
       </c>
       <c r="G34" t="n">
-        <v>6.438193975308641</v>
+        <v>6.28081218106996</v>
       </c>
       <c r="H34" t="inlineStr">
         <is>
@@ -1897,7 +1897,7 @@
         </is>
       </c>
       <c r="I34" t="n">
-        <v>0.5075706</v>
+        <v>0.5074682</v>
       </c>
     </row>
     <row r="35">
@@ -1923,16 +1923,16 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>0.031168 0.071671 0.104468 0.126938 0.123913 0.110148 0.125392 0.125625 0.103462 0.068287 0.021178</t>
+          <t>0.031182 0.071535 0.104612 0.12705 0.123831 0.11006 0.125322 0.125771 0.103558 0.0681 0.021057</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>0.03361464740380526 -0.240022886568445 -1.3561722214275482 -0.09955657273637565 0.28822772135602764 -0.5954799027320842 -0.3056787297954513 -0.22099842654842206 0.9124588756973245 2.151909598054642 1.1839507938778429</t>
+          <t>0.03561722214275535 -0.2594764697468168 -1.3355743098269202 -0.08353597482477489 0.2764983550278916 -0.6080675153769118 -0.31569160349020375 -0.20011443284222735 0.9261908167644106 2.125160921184379 1.166642826491203</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>9.352842460608105</v>
+        <v>9.180431893952129</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
@@ -1940,7 +1940,7 @@
         </is>
       </c>
       <c r="I35" t="n">
-        <v>0.4993599</v>
+        <v>0.4991795999999999</v>
       </c>
     </row>
     <row r="36">
@@ -1966,16 +1966,16 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>0.454762 0.056274 0.357342 0.031139 0.09906 0.004754 0.009103 8.1e-05</t>
+          <t>0.454775 0.056113 0.357334 0.031044 0.099151 0.004739 0.00912 8e-05</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>-0.027555555555558442 0.3696296296296292 -0.3235555555555584 0.3299259259259259 0.9374814814814816 0.24977777777777785 0.3291851851851852 -0.010814814814814815</t>
+          <t>-0.025629629629634703 0.3457777777777782 -0.32474074074074477 0.3158518518518516 0.9509629629629641 0.24755555555555558 0.33170370370370367 -0.010962962962962963</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>1.40066499862826</v>
+        <v>1.401199934156384</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
@@ -1983,7 +1983,7 @@
         </is>
       </c>
       <c r="I36" t="n">
-        <v>0.1913671428571429</v>
+        <v>0.191356</v>
       </c>
     </row>
     <row r="37">
@@ -2009,16 +2009,16 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>0.551539 0.04638 0.309086 0.014368 0.043066 0.000384</t>
+          <t>0.551424 0.046256 0.3093 0.014326 0.043135 0.000379</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>0.7068263473053847 -2.691137724550898 -0.7513772455089757 -0.929940119760479 -0.4511377245508982 -0.09604790419161677</t>
+          <t>0.6930538922155672 -2.7059880239520955 -0.7257485029940065 -0.9349700598802395 -0.442874251497006 -0.09664670658682635</t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>9.38393257556741</v>
+        <v>9.409052974290928</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
@@ -2026,7 +2026,7 @@
         </is>
       </c>
       <c r="I37" t="n">
-        <v>0.176368</v>
+        <v>0.1764538</v>
       </c>
     </row>
     <row r="38">
@@ -2052,16 +2052,16 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>0.504529 0.021502 0.481645 0.005901 0.013586 0.000176 0.0</t>
+          <t>0.504499 0.021962 0.481655 0.005985 0.01342 0.000176 0.0</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>-0.04541116589788358 0.6920629871162717 -0.01940512167965818 0.4526006044218228 1.0804835374582473 0.013997136949260379 -7.95291872117067e-05</t>
+          <t>-0.04779704151423276 0.7286464132336566 -0.01860982980754032 0.45928105614760617 1.067281692381104 0.013997136949260379 -7.95291872117067e-05</t>
         </is>
       </c>
       <c r="G38" t="n">
-        <v>1.85387781888086</v>
+        <v>1.883781704056854</v>
       </c>
       <c r="H38" t="inlineStr">
         <is>
@@ -2069,7 +2069,7 @@
         </is>
       </c>
       <c r="I38" t="n">
-        <v>0.1762865</v>
+        <v>0.1762978333333333</v>
       </c>
     </row>
     <row r="39">
@@ -2095,16 +2095,16 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>0.471751 0.190733 0.235934 0.07241 0.032521 0.005766</t>
+          <t>0.471745 0.190842 0.235815 0.072504 0.032538 0.005778</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>-0.053777777777778105 1.006518518518522 -1.0777777777777784 1.1045925925925932 0.20785185185185207 0.162962962962963</t>
+          <t>-0.05466666666665966 1.0226666666666697 -1.0954074074074092 1.1185185185185187 0.21037037037037 0.16474074074074077</t>
         </is>
       </c>
       <c r="G39" t="n">
-        <v>3.467460631001381</v>
+        <v>3.571231824417019</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
@@ -2112,7 +2112,7 @@
         </is>
       </c>
       <c r="I39" t="n">
-        <v>0.207749</v>
+        <v>0.2078052</v>
       </c>
     </row>
     <row r="40">
@@ -2138,16 +2138,16 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>0.748542 0.030972 0.214114 0.001912</t>
+          <t>0.748502 0.030906 0.214279 0.001886</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>0.7250370370370467 1.2263703703703706 -2.7128888888888882 0.10074074074074076</t>
+          <t>0.7191111111111148 1.2165925925925927 -2.688444444444444 0.0968888888888889</t>
         </is>
       </c>
       <c r="G40" t="n">
-        <v>9.399577810699601</v>
+        <v>9.234339314128947</v>
       </c>
       <c r="H40" t="inlineStr">
         <is>
@@ -2155,7 +2155,7 @@
         </is>
       </c>
       <c r="I40" t="n">
-        <v>0.1549786666666667</v>
+        <v>0.1550406666666667</v>
       </c>
     </row>
     <row r="41">
@@ -2181,16 +2181,16 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>0.413326 0.220123 0.235758 0.092774 0.037828 0.008961 0.00066</t>
+          <t>0.413324 0.220157 0.2357 0.092841 0.037855 0.008972 0.000661</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>0.16088888888889355 -2.4937777777777757 1.5157037037037022 0.9416296296296297 0.9192592592592596 0.3317037037037038 0.021629629629629627</t>
+          <t>0.16059259259259695 -2.488740740740742 1.5071111111111093 0.9515555555555574 0.9232592592592594 0.3333333333333335 0.021777777777777778</t>
         </is>
       </c>
       <c r="G41" t="n">
-        <v>10.38436968998627</v>
+        <v>10.3604553744856</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
@@ -2198,7 +2198,7 @@
         </is>
       </c>
       <c r="I41" t="n">
-        <v>0.1950063333333333</v>
+        <v>0.1950543333333333</v>
       </c>
     </row>
     <row r="42">
@@ -2224,16 +2224,16 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>0.664444 0.122635 0.183869 0.028537 0.003175</t>
+          <t>0.664444 0.12263 0.183868 0.028551 0.003188</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>0.0031111111111183343 -0.07125925925926062 0.01688888888888933 0.08562962962962943 0.35970370370370364</t>
+          <t>0.0031111111111183343 -0.07200000000000005 0.016740740740741035 0.08770370370370352 0.3616296296296296</t>
         </is>
       </c>
       <c r="G42" t="n">
-        <v>0.1420919835390948</v>
+        <v>0.1439418600823045</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
@@ -2241,7 +2241,7 @@
         </is>
       </c>
       <c r="I42" t="n">
-        <v>0.147171</v>
+        <v>0.14719275</v>
       </c>
     </row>
     <row r="43">
@@ -2267,16 +2267,16 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>0.436023 0.162065 0.24231 0.080965 0.04933 0.010345 0.00267</t>
+          <t>0.436014 0.162194 0.242177 0.081113 0.049356 0.010378 0.002675</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>-0.048739807264639494 0.7495058067704458 -0.2293674326661721 -0.15072893501359103 -0.5709167284408203 -0.29256239189523103 -0.4636150234741783</t>
+          <t>-0.049295774647885184 0.7574746725969851 -0.2375833951074863 -0.14158636026686447 -0.569310600444774 -0.29052384482332594 -0.4633061527057079</t>
         </is>
       </c>
       <c r="G43" t="n">
-        <v>1.265940708169004</v>
+        <v>1.275861775393145</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
@@ -2284,7 +2284,7 @@
         </is>
       </c>
       <c r="I43" t="n">
-        <v>0.1924408333333333</v>
+        <v>0.1925418333333333</v>
       </c>
     </row>
     <row r="44">
@@ -2310,16 +2310,16 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>0.427275 0.217864 0.231917 0.091248 0.037206 0.008813 0.000649</t>
+          <t>0.427273 0.217895 0.231858 0.091313 0.037232 0.008824 0.00065</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>0.07644444444444688 -1.1694814814814791 0.0974814814814844 1.7281481481481473 1.0391111111111115 0.3503703703703704 0.09599999999999999</t>
+          <t>0.07614814814815028 -1.1648888888888862 0.08874074074074315 1.7377777777777785 1.042962962962963 0.3520000000000001 0.09614814814814814</t>
         </is>
       </c>
       <c r="G44" t="n">
-        <v>5.58125664746227</v>
+        <v>5.611431396433469</v>
       </c>
       <c r="H44" t="inlineStr">
         <is>
@@ -2327,7 +2327,7 @@
         </is>
       </c>
       <c r="I44" t="n">
-        <v>0.1920375</v>
+        <v>0.192083</v>
       </c>
     </row>
     <row r="45">
@@ -2353,16 +2353,16 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>0.705676 0.038767 0.278973 0.000765</t>
+          <t>0.705682 0.038612 0.278996 0.000749</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>-0.04421715184893985 1.3480199318122215 -0.07563598216627322 0.04012588512981904</t>
+          <t>-0.04390243902438902 1.3398898505114083 -0.07442958300550767 0.039286650931025444</t>
         </is>
       </c>
       <c r="G45" t="n">
-        <v>1.826443781536367</v>
+        <v>1.804315439423524</v>
       </c>
       <c r="H45" t="inlineStr">
         <is>
@@ -2370,7 +2370,7 @@
         </is>
       </c>
       <c r="I45" t="n">
-        <v>0.1996693333333334</v>
+        <v>0.199617</v>
       </c>
     </row>
     <row r="46">
@@ -2396,16 +2396,16 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>0.540757 0.048246 0.410371 0.015563 0.066964 0.000421 1e-06</t>
+          <t>0.540768 0.048067 0.41048 0.015509 0.06666 0.000411 1e-06</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>-0.190081973865754 2.9165652138625107 -0.7004301598896214 1.1664637610583557 3.4547520493466433 0.03416930443957471 8.116224332440549e-05</t>
+          <t>-0.1891891891891869 2.902037172307442 -0.6915834753672592 1.1620809999188377 3.4300787273760243 0.03335768200633066 8.116224332440549e-05</t>
         </is>
       </c>
       <c r="G46" t="n">
-        <v>22.33020318866501</v>
+        <v>22.05288507006733</v>
       </c>
       <c r="H46" t="inlineStr">
         <is>
@@ -2413,7 +2413,7 @@
         </is>
       </c>
       <c r="I46" t="n">
-        <v>0.1976073333333333</v>
+        <v>0.1973758333333333</v>
       </c>
     </row>
     <row r="47">
@@ -2439,16 +2439,16 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>0.621638 0.150501 0.192104 0.036675 0.006841</t>
+          <t>0.621638 0.150494 0.192101 0.036701 0.006859</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>0.010189604024255288 -0.2325551399458273 0.022571907648653227 0.5414678189088095 0.6590997033406423</t>
+          <t>0.010189604024255288 -0.2334580162517743 0.022184960660390232 0.5448213594737519 0.6614213852702179</t>
         </is>
       </c>
       <c r="G47" t="n">
-        <v>0.7822950300178797</v>
+        <v>0.7894072084934891</v>
       </c>
       <c r="H47" t="inlineStr">
         <is>
@@ -2456,7 +2456,7 @@
         </is>
       </c>
       <c r="I47" t="n">
-        <v>0.1680245</v>
+        <v>0.16805875</v>
       </c>
     </row>
     <row r="48">
@@ -2482,16 +2482,16 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>0.869942 0.026418 0.124625 0.000342</t>
+          <t>0.869941 0.026449 0.12462 0.000335</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>-0.00875941637260097 0.2668118227094126 0.0045423830617914536 0.0042796005706134095</t>
+          <t>-0.008771929824562189 0.2671997397201992 0.004479815801987102 0.004192006406887404</t>
         </is>
       </c>
       <c r="G48" t="n">
-        <v>0.07130422433763167</v>
+        <v>0.07151028932672437</v>
       </c>
       <c r="H48" t="inlineStr">
         <is>
@@ -2499,7 +2499,7 @@
         </is>
       </c>
       <c r="I48" t="n">
-        <v>0.09223133333333335</v>
+        <v>0.09223133333333332</v>
       </c>
     </row>
     <row r="49">
@@ -2525,16 +2525,16 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>0.496128 0.020974 0.480694 0.005889 0.01356 0.000176 0.0</t>
+          <t>0.496098 0.021433 0.480704 0.005973 0.013394 0.000176 0.0</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>-0.07155555555555722 1.0919999999999999 -0.02399999999999933 0.5354074074074074 1.548 0.0057777777777777775 -0.5047407407407407</t>
+          <t>-0.0760000000000061 1.1600000000000001 -0.022518518518516367 0.5478518518518518 1.5234074074074075 0.0057777777777777775 -0.5047407407407407</t>
         </is>
       </c>
       <c r="G49" t="n">
-        <v>4.135921887517147</v>
+        <v>4.227591462277093</v>
       </c>
       <c r="H49" t="inlineStr">
         <is>
@@ -2542,7 +2542,7 @@
         </is>
       </c>
       <c r="I49" t="n">
-        <v>0.1758581666666667</v>
+        <v>0.1758693333333333</v>
       </c>
     </row>
     <row r="50">
@@ -2568,16 +2568,16 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>0.467054 0.191585 0.237509 0.072896 0.032739 0.005805</t>
+          <t>0.467048 0.191696 0.237393 0.072992 0.032757 0.005817</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>-0.01570370370370296 0.29955555555555496 -0.5402962962962979 0.9088888888888891 0.3448888888888884 0.12681481481481482</t>
+          <t>-0.01659259259259274 0.3159999999999994 -0.5574814814814839 0.9231111111111112 0.3475555555555557 0.12859259259259256</t>
         </is>
       </c>
       <c r="G50" t="n">
-        <v>1.343009580246915</v>
+        <v>1.400381958847739</v>
       </c>
       <c r="H50" t="inlineStr">
         <is>
@@ -2585,7 +2585,7 @@
         </is>
       </c>
       <c r="I50" t="n">
-        <v>0.2090544</v>
+        <v>0.2091142</v>
       </c>
     </row>
     <row r="51">
@@ -2611,16 +2611,16 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>0.467005 0.191823 0.237853 0.073002 0.032787 0.005813</t>
+          <t>0.466999 0.191933 0.237735 0.073097 0.032804 0.005825</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>-0.04518518518518514 0.8478518518518527 -0.9325925925925919 0.9896296296296284 0.21955555555555514 0.14785185185185182</t>
+          <t>-0.04607407407407492 0.8641481481481489 -0.9500740740740744 1.0037037037037022 0.22207407407407412 0.1496296296296297</t>
         </is>
       </c>
       <c r="G51" t="n">
-        <v>2.640055023319614</v>
+        <v>2.730642633744855</v>
       </c>
       <c r="H51" t="inlineStr">
         <is>
@@ -2628,7 +2628,7 @@
         </is>
       </c>
       <c r="I51" t="n">
-        <v>0.2093496</v>
+        <v>0.209407</v>
       </c>
     </row>
     <row r="52">
@@ -2654,16 +2654,16 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>0.78114 0.213079 0.005771</t>
+          <t>0.78114 0.213079 0.005781</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>0.0 0.0 -0.0013042911177774347</t>
+          <t>0.0 0.0 0.0</t>
         </is>
       </c>
       <c r="G52" t="n">
-        <v>1.70117531991311e-06</v>
+        <v>0</v>
       </c>
       <c r="H52" t="inlineStr">
         <is>
@@ -2671,7 +2671,7 @@
         </is>
       </c>
       <c r="I52" t="n">
-        <v>0.1123105</v>
+        <v>0.1123205</v>
       </c>
     </row>
     <row r="53">
@@ -2697,16 +2697,16 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>0.726558 0.036999 0.235203 0.000645</t>
+          <t>0.726562 0.036868 0.23521 0.000631</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>0.006666666666677446 -0.20133333333333422 0.01096296296296159 0.09555555555555555</t>
+          <t>0.0072592592592706316 -0.22074074074074151 0.011999999999999665 0.09348148148148148</t>
         </is>
       </c>
       <c r="G53" t="n">
-        <v>0.04983060631001419</v>
+        <v>0.05766195884773713</v>
       </c>
       <c r="H53" t="inlineStr">
         <is>
@@ -2714,7 +2714,7 @@
         </is>
       </c>
       <c r="I53" t="n">
-        <v>0.16978</v>
+        <v>0.169727</v>
       </c>
     </row>
     <row r="54">
@@ -2740,16 +2740,16 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>0.367128 0.425296 0.152386 0.05095 0.013344 0.000963 3e-06</t>
+          <t>0.367042 0.425346 0.152432 0.051024 0.013323 0.00095 2e-06</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>0.488148148148147 -0.5157037037037054 -0.09570370370370485 0.9152592592592597 0.5958518518518517 0.1037037037037037 0.00029629629629629635</t>
+          <t>0.4754074074074018 -0.5082962962962989 -0.08888888888888732 0.9262222222222223 0.5927407407407407 0.10177777777777777 0.00014814814814814815</t>
         </is>
       </c>
       <c r="G54" t="n">
-        <v>1.716891610425241</v>
+        <v>1.711866491083673</v>
       </c>
       <c r="H54" t="inlineStr">
         <is>
@@ -2757,7 +2757,7 @@
         </is>
       </c>
       <c r="I54" t="n">
-        <v>0.1568545</v>
+        <v>0.1568893333333334</v>
       </c>
     </row>
     <row r="55">
@@ -2783,16 +2783,16 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>0.500079 0.110986 0.290335 0.051826 0.043263 0.00578 0.000389</t>
+          <t>0.500496 0.110738 0.289741 0.051706 0.043225 0.005773 0.000391</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>-0.06755555555554088 0.12740740740740736 0.0002962962962965926 0.825185185185185 -0.54637037037037 0.06666666666666678 -0.011851851851851851</t>
+          <t>-0.005777777777762997 0.09066666666666688 -0.08770370370370095 0.8074074074074079 -0.552 0.06562962962962973 -0.011555555555555555</t>
         </is>
       </c>
       <c r="G55" t="n">
-        <v>1.004832570644716</v>
+        <v>0.9769972674897122</v>
       </c>
       <c r="H55" t="inlineStr">
         <is>
@@ -2800,7 +2800,7 @@
         </is>
       </c>
       <c r="I55" t="n">
-        <v>0.1752366666666667</v>
+        <v>0.1749081666666666</v>
       </c>
     </row>
     <row r="56">
@@ -2826,16 +2826,16 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>0.467333 0.056888 0.345339 0.029333 0.094115 0.003993 0.008495</t>
+          <t>0.467345 0.056707 0.345329 0.029249 0.094208 0.003986 0.008512</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>0.043111111111109 -0.6494814814814813 -0.29037037037037294 0.04740740740740753 1.194666666666667 0.16148148148148145 0.30740740740740746</t>
+          <t>0.04488888888888855 -0.6762962962962963 -0.2918518518518559 0.03496296296296298 1.2084444444444442 0.16044444444444442 0.30992592592592594</t>
         </is>
       </c>
       <c r="G56" t="n">
-        <v>2.058051204389577</v>
+        <v>2.127926079561044</v>
       </c>
       <c r="H56" t="inlineStr">
         <is>
@@ -2843,7 +2843,7 @@
         </is>
       </c>
       <c r="I56" t="n">
-        <v>0.2138266666666667</v>
+        <v>0.2138243333333333</v>
       </c>
     </row>
     <row r="57">
@@ -2869,16 +2869,16 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>0.407275 0.189974 0.24889 0.097595 0.055103 0.012719 0.003521</t>
+          <t>0.407269 0.190073 0.248754 0.097743 0.055107 0.012753 0.003522</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>0.02014814814815185 -0.2905185185185171 -0.6706666666666672 1.8838518518518526 0.4185185185185187 0.42503703703703705 0.44725925925925925</t>
+          <t>0.019259259259262074 -0.27585185185185224 -0.6908148148148149 1.9057777777777778 0.4191111111111119 0.4300740740740742 0.4474074074074074</t>
         </is>
       </c>
       <c r="G57" t="n">
-        <v>4.639353613168728</v>
+        <v>4.746470430727024</v>
       </c>
       <c r="H57" t="inlineStr">
         <is>
@@ -2886,7 +2886,7 @@
         </is>
       </c>
       <c r="I57" t="n">
-        <v>0.2142786666666667</v>
+        <v>0.2143558333333333</v>
       </c>
     </row>
     <row r="58">
@@ -2912,16 +2912,16 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>0.629146 0.139842 0.192491 0.033735 0.005849</t>
+          <t>0.629147 0.139835 0.192491 0.033756 0.005857</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>0.0017777777777795557 -0.04148148148148185 0.0010370370370380742 0.11896296296296269 0.07718518518518515</t>
+          <t>0.001925925925931964 -0.04251851851851992 0.0010370370370380742 0.12207407407407384 0.07837037037037037</t>
         </is>
       </c>
       <c r="G58" t="n">
-        <v>0.02183468861454043</v>
+        <v>0.02285660356652958</v>
       </c>
       <c r="H58" t="inlineStr">
         <is>
@@ -2929,7 +2929,7 @@
         </is>
       </c>
       <c r="I58" t="n">
-        <v>0.16235625</v>
+        <v>0.16237825</v>
       </c>
     </row>
     <row r="59">
@@ -2955,16 +2955,16 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>0.52638 0.238141 0.173555 0.065102 0.007622 0.000423</t>
+          <t>0.526385 0.238057 0.173629 0.065132 0.007635 0.000427</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>0.08483540205072351 -1.5878035617916921 1.62245008094981 0.763410685375067 0.2827846735024285 0.04565569347004857</t>
+          <t>0.08537506745817443 -1.5968699406368083 1.6304371289800332 0.7666486778197515 0.2841878035617917 0.04608742579600648</t>
         </is>
       </c>
       <c r="G59" t="n">
-        <v>5.825508949912471</v>
+        <v>5.886244694722096</v>
       </c>
       <c r="H59" t="inlineStr">
         <is>
@@ -2972,7 +2972,7 @@
         </is>
       </c>
       <c r="I59" t="n">
-        <v>0.162632</v>
+        <v>0.1626772</v>
       </c>
     </row>
     <row r="60">
@@ -2998,16 +2998,16 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>0.490963 0.186224 0.228024 0.06997 0.031425 0.005571</t>
+          <t>0.490957 0.186335 0.227917 0.070063 0.031442 0.005583</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>0.06311111111110844 -1.1631111111111108 0.4140740740740729 0.7391111111111122 1.1506666666666672 0.6001481481481483</t>
+          <t>0.06222222222221866 -1.1466666666666663 0.39822222222222164 0.7528888888888894 1.153185185185185 0.601925925925926</t>
         </is>
       </c>
       <c r="G60" t="n">
-        <v>3.758764620027435</v>
+        <v>3.736289558299039</v>
       </c>
       <c r="H60" t="inlineStr">
         <is>
@@ -3015,7 +3015,7 @@
         </is>
       </c>
       <c r="I60" t="n">
-        <v>0.2011474</v>
+        <v>0.2012082</v>
       </c>
     </row>
     <row r="61">
@@ -3041,16 +3041,16 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>0.79589 0.022753 0.197062 0.00054</t>
+          <t>0.795888 0.022803 0.197059 0.000529</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>-0.036261491317671916 1.1055924412665985 0.01896067415730284 -0.051200204290091936</t>
+          <t>-0.03638917262512509 1.1087844739530133 0.018769152196119538 -0.05190245148110317</t>
         </is>
       </c>
       <c r="G61" t="n">
-        <v>1.226630510022265</v>
+        <v>1.233773327107511</v>
       </c>
       <c r="H61" t="inlineStr">
         <is>
@@ -3058,7 +3058,7 @@
         </is>
       </c>
       <c r="I61" t="n">
-        <v>0.139499</v>
+        <v>0.1395026666666667</v>
       </c>
     </row>
     <row r="62">
@@ -3084,16 +3084,16 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>0.530761 0.048338 0.324551 0.024059 0.067505 0.004397 0.004096 0.000306 2e-06 0.0</t>
+          <t>0.530756 0.048396 0.324546 0.024067 0.06753 0.004395 0.004097 0.000306 2e-06 0.0</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>0.07970303964141219 -0.7984311528225246 -0.255217817621522 -0.7090628939627399 1.3726012046505105 0.3342204790586916 0.4954475416725031 0.042863146098893405 0.0002801512816921137 0.0</t>
+          <t>0.07900266143717732 -0.790306765653453 -0.2559181958257491 -0.7079422888359713 1.3761030956716636 0.3339403277769995 0.49558761731334916 0.042863146098893405 0.0002801512816921137 0.0</t>
         </is>
       </c>
       <c r="G62" t="n">
-        <v>3.454794192309711</v>
+        <v>3.450122898274303</v>
       </c>
       <c r="H62" t="inlineStr">
         <is>
@@ -3101,7 +3101,7 @@
         </is>
       </c>
       <c r="I62" t="n">
-        <v>0.1209284444444444</v>
+        <v>0.1209471111111111</v>
       </c>
     </row>
     <row r="63">
@@ -3127,16 +3127,16 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>0.538478 0.049302 0.307656 0.022799 0.063959 0.004166 0.003881 0.00029 2e-06 0.0</t>
+          <t>0.538473 0.049357 0.307653 0.022806 0.063984 0.004165 0.003882 0.00029 1e-06 0.0</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>0.13750454710803545 -1.3918697708257546 -0.10722080756639152 -0.7304474354310659 0.6566933430338309 0.3161149508912332 0.23162968352128044 0.026373226627864677 0.0001818843215714805 0.0</t>
+          <t>0.13704983630410375 -1.386867951982539 -0.10749363404874648 -0.7298108403055658 0.6589668970534742 0.31602400873044745 0.2317206256820662 0.026373226627864677 9.094216078574026e-05 0.0</t>
         </is>
       </c>
       <c r="G63" t="n">
-        <v>3.086781416331691</v>
+        <v>3.074862667081821</v>
       </c>
       <c r="H63" t="inlineStr">
         <is>
@@ -3144,7 +3144,7 @@
         </is>
       </c>
       <c r="I63" t="n">
-        <v>0.115001</v>
+        <v>0.1150191111111111</v>
       </c>
     </row>
     <row r="64">
@@ -3170,16 +3170,16 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>0.480632 0.188706 0.232359 0.071307 0.032026 0.005678</t>
+          <t>0.480626 0.188818 0.232248 0.071402 0.032043 0.00569</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>0.03718518518518537 -0.6825185185185185 0.08859259259259485 0.8402962962962958 0.8737777777777779 0.429037037037037</t>
+          <t>0.03629629629629559 -0.6659259259259258 0.0721481481481504 0.8543703703703696 0.8762962962962968 0.43081481481481476</t>
         </is>
       </c>
       <c r="G64" t="n">
-        <v>2.128721163237311</v>
+        <v>2.13342544855967</v>
       </c>
       <c r="H64" t="inlineStr">
         <is>
@@ -3187,7 +3187,7 @@
         </is>
       </c>
       <c r="I64" t="n">
-        <v>0.2047678</v>
+        <v>0.2048284</v>
       </c>
     </row>
     <row r="65">
@@ -3213,16 +3213,16 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>0.758165 0.031169 0.210176 0.001877</t>
+          <t>0.758167 0.031099 0.210179 0.001849</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>-0.018370370370372296 0.5619259259259256 -0.013925925925927517 -0.32414814814814813</t>
+          <t>-0.018074074074067477 0.5515555555555557 -0.013481481481482628 -0.3282962962962963</t>
         </is>
       </c>
       <c r="G65" t="n">
-        <v>0.4213641700960217</v>
+        <v>0.4125004115226337</v>
       </c>
       <c r="H65" t="inlineStr">
         <is>
@@ -3230,7 +3230,7 @@
         </is>
       </c>
       <c r="I65" t="n">
-        <v>0.152384</v>
+        <v>0.1523346666666667</v>
       </c>
     </row>
     <row r="66">
@@ -3256,16 +3256,16 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>0.535929 0.414449 0.074963 0.044061 0.004122 1.1e-05</t>
+          <t>0.53593 0.414433 0.074967 0.044135 0.004067 1.1e-05</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>0.024587500451313957 -0.48835613965411356 1.7410188829115067 1.3183377261075209 0.14882478246741523 -0.08943206845506733</t>
+          <t>0.02462360544463557 -0.48893381954724335 1.741163302884789 1.3210094956132434 0.14683900783478357 -0.08943206845506733</t>
         </is>
       </c>
       <c r="G66" t="n">
-        <v>5.038404285793717</v>
+        <v>5.045938125745228</v>
       </c>
       <c r="H66" t="inlineStr">
         <is>
@@ -3273,7 +3273,7 @@
         </is>
       </c>
       <c r="I66" t="n">
-        <v>0.1426202</v>
+        <v>0.142619</v>
       </c>
     </row>
     <row r="67">
@@ -3299,16 +3299,16 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>0.291435 0.317865 0.288483 0.060508 0.028836 0.003693 0.000156 0.0</t>
+          <t>0.291792 0.317874 0.288158 0.060248 0.028778 0.003646 0.000151 0.0</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>0.19108635097492818 0.30069637883008665 -0.1600278551532049 -1.9598885793871859 0.4844011142061284 -0.13481894150417828 0.021727019498607242 0.0</t>
+          <t>0.24080779944289424 0.30194986072423446 -0.20529247910863166 -1.9961002785515307 0.4763231197771592 -0.14136490250696382 0.02103064066852368 0.0</t>
         </is>
       </c>
       <c r="G67" t="n">
-        <v>4.246997113616436</v>
+        <v>4.423033476617958</v>
       </c>
       <c r="H67" t="inlineStr">
         <is>
@@ -3316,7 +3316,7 @@
         </is>
       </c>
       <c r="I67" t="n">
-        <v>0.1730142857142857</v>
+        <v>0.1727402857142857</v>
       </c>
     </row>
     <row r="68">
@@ -3342,16 +3342,16 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>0.759339 0.078501 0.168591 0.000469</t>
+          <t>0.759366 0.077657 0.16891 0.000512</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>-0.031582025538550634 0.9663709913246911 -0.3078272736134147 0.045618481333463294</t>
+          <t>-0.028950190077004747 0.8841017643045139 -0.2767326250121852 0.049809922994443895</t>
         </is>
       </c>
       <c r="G68" t="n">
-        <v>1.031708993430424</v>
+        <v>0.8615360173266962</v>
       </c>
       <c r="H68" t="inlineStr">
         <is>
@@ -3359,7 +3359,7 @@
         </is>
       </c>
       <c r="I68" t="n">
-        <v>0.13903</v>
+        <v>0.1390043333333333</v>
       </c>
     </row>
     <row r="69">
@@ -3385,16 +3385,16 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>0.52402 0.204231 0.204382 0.052487 0.017072</t>
+          <t>0.524021 0.204216 0.20438 0.052538 0.017079</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>0.006666666666677446 -0.15214814814814817 -0.0044444444444447775 0.5761481481481476 -0.1014814814814812</t>
+          <t>0.006814814814813407 -0.1543703703703685 -0.00474074074074137 0.5837037037037036 -0.10044444444444416</t>
         </is>
       </c>
       <c r="G69" t="n">
-        <v>0.3654584362139913</v>
+        <v>0.3746982277091899</v>
       </c>
       <c r="H69" t="inlineStr">
         <is>
@@ -3402,7 +3402,7 @@
         </is>
       </c>
       <c r="I69" t="n">
-        <v>0.209686</v>
+        <v>0.2097265</v>
       </c>
     </row>
     <row r="70">
@@ -3428,16 +3428,16 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>0.659728 0.115085 0.191161 0.026701 0.001815</t>
+          <t>0.65973 0.115032 0.191181 0.026698 0.001828</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>0.087111111111116 -2.005777777777775 0.9072592592592579 -0.016000000000000066 0.2111111111111111</t>
+          <t>0.08740740740742081 -2.0136296296296288 0.9102222222222197 -0.016444444444444442 0.21303703703703705</t>
         </is>
       </c>
       <c r="G70" t="n">
-        <v>4.898676104252389</v>
+        <v>4.936504032921805</v>
       </c>
       <c r="H70" t="inlineStr">
         <is>
@@ -3445,7 +3445,7 @@
         </is>
       </c>
       <c r="I70" t="n">
-        <v>0.1461925</v>
+        <v>0.1462</v>
       </c>
     </row>
     <row r="71">
@@ -3471,16 +3471,16 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>0.269388 0.266969 0.218018 0.165023 0.057761 0.032175 0.005621 0.001957 0.000195 6e-06 0.0 0.0</t>
+          <t>0.269417 0.266722 0.218047 0.165263 0.057791 0.032292 0.005626 0.001966 0.000195 6e-06 0.0 0.0</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>0.12728310502283477 -1.0383561643835608 -0.41803652968036514 1.63230593607306 0.7422374429223745 0.6138127853881282 0.29691780821917807 0.2065068493150685 0.02226027397260274 0.0006849315068493151 -0.23207762557077624 0.0</t>
+          <t>0.13059360730593994 -1.0665525114155239 -0.41472602739725994 1.6597031963470315 0.7456621004566213 0.6271689497716897 0.2974885844748858 0.20753424657534245 0.02226027397260274 0.0006849315068493151 -0.23207762557077624 0.0</t>
         </is>
       </c>
       <c r="G71" t="n">
-        <v>5.046405556076816</v>
+        <v>5.21648012186985</v>
       </c>
       <c r="H71" t="inlineStr">
         <is>
@@ -3488,7 +3488,7 @@
         </is>
       </c>
       <c r="I71" t="n">
-        <v>0.1490029090909091</v>
+        <v>0.1491237272727272</v>
       </c>
     </row>
     <row r="72">
@@ -3514,16 +3514,16 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>0.50707 0.04604 0.321692 0.023851 0.066928 0.00436 0.004061 0.000303 2e-06 0.0</t>
+          <t>0.507064 0.046097 0.32169 0.023859 0.066953 0.004358 0.004062 0.000303 2e-06 0.0</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>0.3537777777777862 -3.58562962962963 -0.1681481481481477 -1.4081481481481475 1.1072592592592594 -0.306962962962963 0.15629629629629635 0.04488888888888889 0.0002962962962962963 0.0</t>
+          <t>0.3528888888888882 -3.5771851851851855 -0.1684444444444443 -1.4069629629629623 1.1109629629629627 -0.3072592592592593 0.15644444444444439 0.04488888888888889 0.0002962962962962963 0.0</t>
         </is>
       </c>
       <c r="G72" t="n">
-        <v>16.3397465240055</v>
+        <v>16.28383964883401</v>
       </c>
       <c r="H72" t="inlineStr">
         <is>
@@ -3531,7 +3531,7 @@
         </is>
       </c>
       <c r="I72" t="n">
-        <v>0.1196657777777778</v>
+        <v>0.119685</v>
       </c>
     </row>
     <row r="73">
@@ -3557,16 +3557,16 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>0.577392 0.048554 0.323574 0.015042 0.045085 0.000402</t>
+          <t>0.57771 0.048408 0.323041 0.014962 0.045051 0.000396</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>-0.1114074074074037 1.1986666666666668 0.016296296296296146 0.501925925925926 -0.14888888888888874 0.03214814814814815</t>
+          <t>-0.06429629629630303 1.177037037037037 -0.06266666666665943 0.4900740740740741 -0.15392592592592566 0.03125925925925926</t>
         </is>
       </c>
       <c r="G73" t="n">
-        <v>1.724609997256515</v>
+        <v>1.658320241426612</v>
       </c>
       <c r="H73" t="inlineStr">
         <is>
@@ -3574,7 +3574,7 @@
         </is>
       </c>
       <c r="I73" t="n">
-        <v>0.1846356</v>
+        <v>0.184312</v>
       </c>
     </row>
     <row r="74">
@@ -3600,16 +3600,16 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>0.208556 0.363866 0.272321 0.123069 0.041914 0.010848 0.001821 0.000165 6e-06 0.0 0.0</t>
+          <t>0.208578 0.363655 0.272442 0.12329 0.042023 0.010874 0.001825 0.000166 6e-06 0.0 0.0</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>0.1886294134000552 -1.8031693077564614 1.568251320544893 1.0496246872393664 1.268001112037809 0.6501251042535446 0.19154851264943007 0.022935779816513763 0.0008340283569641369 0.0 0.0</t>
+          <t>0.19168751737559342 -1.8324993049763694 1.5850708924103414 1.0803447317208787 1.2831526271893239 0.6537392271337226 0.19210453155407284 0.02307478454267445 0.0008340283569641369 0.0 0.0</t>
         </is>
       </c>
       <c r="G74" t="n">
-        <v>8.915831846094804</v>
+        <v>9.185685214464929</v>
       </c>
       <c r="H74" t="inlineStr">
         <is>
@@ -3617,7 +3617,7 @@
         </is>
       </c>
       <c r="I74" t="n">
-        <v>0.151174</v>
+        <v>0.1513031</v>
       </c>
     </row>
   </sheetData>

</xml_diff>